<commit_message>
Test Automation Framework - git CI/CD
</commit_message>
<xml_diff>
--- a/config/Master_Test_Template.xlsx
+++ b/config/Master_Test_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gomat\PycharmProjects\test_automation_project\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A4952\PycharmProjects\test_automation_project\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B381940-95DF-43B1-9E93-319D5B1847FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C3BB8D-F1C8-4A71-BC5D-8582DB8507FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10296" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_validation" sheetId="1" r:id="rId1"/>
@@ -210,9 +210,6 @@
     <t>contact_info_schema.json</t>
   </si>
   <si>
-    <t>Contact_info.csv</t>
-  </si>
-  <si>
     <t>singleline.json</t>
   </si>
   <si>
@@ -271,18 +268,35 @@
   </si>
   <si>
     <t>transaction_amt</t>
+  </si>
+  <si>
+    <t>Contact_info_21092024.csv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="33">
+  <fonts count="35">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -527,100 +541,112 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -628,14 +654,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -933,10 +953,10 @@
   <dimension ref="A1:W39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
@@ -949,7 +969,7 @@
     <col min="6" max="6" width="15.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="30.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.77734375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="90.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
@@ -960,7 +980,7 @@
     <col min="17" max="17" width="26.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="7.77734375" style="2" bestFit="1" customWidth="1"/>
@@ -980,16 +1000,16 @@
       <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="H1" s="31" t="s">
         <v>22</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -998,34 +1018,34 @@
       <c r="J1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="30" t="s">
+      <c r="K1" s="29" t="s">
         <v>49</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="8" t="s">
         <v>24</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="37" t="s">
+      <c r="O1" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="38" t="s">
+      <c r="Q1" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="R1" s="9" t="s">
         <v>1</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="T1" s="42" t="s">
+      <c r="T1" s="41" t="s">
         <v>21</v>
       </c>
       <c r="U1" s="2" t="s">
@@ -1039,14 +1059,14 @@
       </c>
     </row>
     <row r="2" spans="1:23">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>0</v>
@@ -1063,8 +1083,8 @@
       <c r="H2" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="I2" s="34" t="s">
-        <v>64</v>
+      <c r="I2" s="33" t="s">
+        <v>63</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>0</v>
@@ -1075,35 +1095,35 @@
       <c r="L2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="26" t="s">
+      <c r="M2" s="25" t="s">
         <v>17</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="P2" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q2" s="38" t="s">
+      <c r="O2" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="P2" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="R2" s="20"/>
+      <c r="Q2" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="R2" s="19"/>
       <c r="S2" s="1" t="s">
-        <v>67</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:23">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="25" t="s">
         <v>40</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>0</v>
@@ -1120,8 +1140,8 @@
       <c r="H3" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="I3" s="34" t="s">
-        <v>64</v>
+      <c r="I3" s="33" t="s">
+        <v>63</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>0</v>
@@ -1132,35 +1152,35 @@
       <c r="L3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="26" t="s">
+      <c r="M3" s="25" t="s">
         <v>17</v>
       </c>
       <c r="N3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="O3" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="P3" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q3" s="38" t="s">
+      <c r="O3" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="P3" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="R3" s="20"/>
+      <c r="Q3" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="R3" s="19"/>
       <c r="S3" s="1" t="s">
-        <v>67</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:23">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="25" t="s">
         <v>41</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>0</v>
@@ -1177,8 +1197,8 @@
       <c r="H4" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="I4" s="34" t="s">
-        <v>64</v>
+      <c r="I4" s="33" t="s">
+        <v>63</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>0</v>
@@ -1189,35 +1209,35 @@
       <c r="L4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="26" t="s">
+      <c r="M4" s="25" t="s">
         <v>17</v>
       </c>
       <c r="N4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="O4" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="P4" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q4" s="38" t="s">
+      <c r="O4" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="P4" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="R4" s="20"/>
+      <c r="Q4" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="R4" s="19"/>
       <c r="S4" s="1" t="s">
-        <v>67</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:23">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="25" t="s">
         <v>42</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>0</v>
@@ -1234,8 +1254,8 @@
       <c r="H5" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="I5" s="34" t="s">
-        <v>64</v>
+      <c r="I5" s="33" t="s">
+        <v>63</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>0</v>
@@ -1246,35 +1266,35 @@
       <c r="L5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="M5" s="26" t="s">
+      <c r="M5" s="25" t="s">
         <v>17</v>
       </c>
       <c r="N5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="O5" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="P5" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q5" s="38" t="s">
+      <c r="O5" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="P5" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="R5" s="20"/>
+      <c r="Q5" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="R5" s="19"/>
       <c r="S5" s="1" t="s">
-        <v>67</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:23">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="25" t="s">
         <v>43</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>0</v>
@@ -1291,8 +1311,8 @@
       <c r="H6" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="I6" s="34" t="s">
-        <v>64</v>
+      <c r="I6" s="33" t="s">
+        <v>63</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>0</v>
@@ -1303,35 +1323,35 @@
       <c r="L6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="M6" s="26" t="s">
+      <c r="M6" s="25" t="s">
         <v>17</v>
       </c>
       <c r="N6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="O6" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="P6" s="37" t="s">
+      <c r="O6" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="P6" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q6" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="R6" s="19"/>
+      <c r="S6" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23">
+      <c r="A7" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="Q6" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="R6" s="20"/>
-      <c r="S6" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23">
-      <c r="A7" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>77</v>
-      </c>
       <c r="C7" s="3" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>0</v>
@@ -1348,8 +1368,8 @@
       <c r="H7" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="I7" s="34" t="s">
-        <v>64</v>
+      <c r="I7" s="33" t="s">
+        <v>63</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>0</v>
@@ -1360,35 +1380,35 @@
       <c r="L7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="M7" s="26" t="s">
+      <c r="M7" s="25" t="s">
         <v>17</v>
       </c>
       <c r="N7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="O7" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="P7" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q7" s="38" t="s">
+      <c r="O7" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="P7" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="R7" s="20"/>
+      <c r="Q7" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="R7" s="19"/>
       <c r="S7" s="1" t="s">
-        <v>67</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:23">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="25" t="s">
         <v>50</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>0</v>
@@ -1405,8 +1425,8 @@
       <c r="H8" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="I8" s="34" t="s">
-        <v>64</v>
+      <c r="I8" s="33" t="s">
+        <v>63</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>0</v>
@@ -1417,35 +1437,35 @@
       <c r="L8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="M8" s="26" t="s">
+      <c r="M8" s="25" t="s">
         <v>17</v>
       </c>
       <c r="N8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="O8" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="P8" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q8" s="38" t="s">
+      <c r="O8" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="P8" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="R8" s="20"/>
+      <c r="Q8" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="R8" s="19"/>
       <c r="S8" s="1" t="s">
-        <v>67</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:23">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="39" t="s">
         <v>53</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>0</v>
@@ -1462,8 +1482,8 @@
       <c r="H9" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="I9" s="34" t="s">
-        <v>64</v>
+      <c r="I9" s="33" t="s">
+        <v>63</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>0</v>
@@ -1474,35 +1494,35 @@
       <c r="L9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="M9" s="26" t="s">
+      <c r="M9" s="25" t="s">
         <v>17</v>
       </c>
       <c r="N9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="O9" s="39" t="s">
+      <c r="O9" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="P9" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q9" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="R9" s="19"/>
+      <c r="S9" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
+      <c r="A10" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="P9" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q9" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="R9" s="20"/>
-      <c r="S9" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23">
-      <c r="A10" s="41" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>80</v>
-      </c>
       <c r="C10" s="3" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>0</v>
@@ -1519,8 +1539,8 @@
       <c r="H10" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="I10" s="34" t="s">
-        <v>64</v>
+      <c r="I10" s="33" t="s">
+        <v>63</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>0</v>
@@ -1531,29 +1551,29 @@
       <c r="L10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="M10" s="26" t="s">
+      <c r="M10" s="25" t="s">
         <v>17</v>
       </c>
       <c r="N10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="O10" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="P10" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q10" s="38" t="s">
+      <c r="O10" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="P10" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="R10" s="20"/>
+      <c r="Q10" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="R10" s="19"/>
       <c r="S10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="T10" s="42" t="s">
-        <v>81</v>
-      </c>
-      <c r="U10" s="42"/>
+        <v>66</v>
+      </c>
+      <c r="T10" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="U10" s="41"/>
       <c r="V10" s="2">
         <v>5</v>
       </c>
@@ -1562,14 +1582,14 @@
       </c>
     </row>
     <row r="11" spans="1:23">
-      <c r="A11" s="41" t="s">
-        <v>72</v>
+      <c r="A11" s="40" t="s">
+        <v>71</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>0</v>
@@ -1586,8 +1606,8 @@
       <c r="H11" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="I11" s="34" t="s">
-        <v>64</v>
+      <c r="I11" s="33" t="s">
+        <v>63</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>0</v>
@@ -1598,35 +1618,35 @@
       <c r="L11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="M11" s="26" t="s">
+      <c r="M11" s="25" t="s">
         <v>17</v>
       </c>
       <c r="N11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="O11" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="P11" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q11" s="38" t="s">
+      <c r="O11" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="P11" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="R11" s="20"/>
+      <c r="Q11" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="R11" s="19"/>
       <c r="S11" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:23">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="25" t="s">
         <v>44</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>45</v>
@@ -1637,14 +1657,14 @@
       <c r="F12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="H12" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" s="35" t="s">
-        <v>65</v>
+      <c r="G12" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="34" t="s">
+        <v>64</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>45</v>
@@ -1655,35 +1675,35 @@
       <c r="L12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="M12" s="26" t="s">
+      <c r="M12" s="25" t="s">
         <v>17</v>
       </c>
       <c r="N12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="O12" s="26" t="s">
+      <c r="O12" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="P12" s="27" t="s">
+      <c r="P12" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="Q12" s="28" t="s">
+      <c r="Q12" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="R12" s="12"/>
+      <c r="R12" s="11"/>
       <c r="S12" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:23">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="30" t="s">
         <v>50</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>51</v>
@@ -1694,14 +1714,14 @@
       <c r="F13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="I13" s="35" t="s">
-        <v>66</v>
+      <c r="G13" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="34" t="s">
+        <v>65</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>52</v>
@@ -1712,28 +1732,28 @@
       <c r="L13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="M13" s="26" t="s">
+      <c r="M13" s="25" t="s">
         <v>17</v>
       </c>
       <c r="N13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="O13" s="26" t="s">
+      <c r="O13" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="P13" s="27" t="s">
+      <c r="P13" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="Q13" s="28" t="s">
+      <c r="Q13" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="R13" s="12"/>
+      <c r="R13" s="11"/>
       <c r="S13" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:23">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="30" t="s">
         <v>53</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -1751,13 +1771,13 @@
       <c r="F14" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G14" s="33" t="s">
+      <c r="G14" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="H14" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="I14" s="36" t="s">
+      <c r="H14" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="35" t="s">
         <v>56</v>
       </c>
       <c r="J14" s="3" t="s">
@@ -1769,29 +1789,29 @@
       <c r="L14" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="M14" s="26" t="s">
+      <c r="M14" s="25" t="s">
         <v>17</v>
       </c>
       <c r="N14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="O14" s="41" t="s">
+      <c r="O14" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="P14" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="P14" s="37" t="s">
+      <c r="Q14" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="R14" s="11"/>
+      <c r="S14" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23">
+      <c r="A15" s="36" t="s">
         <v>69</v>
-      </c>
-      <c r="Q14" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="R14" s="12"/>
-      <c r="S14" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23">
-      <c r="A15" s="37" t="s">
-        <v>70</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>29</v>
@@ -1808,13 +1828,13 @@
       <c r="F15" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G15" s="33" t="s">
+      <c r="G15" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="H15" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" s="36" t="s">
+      <c r="H15" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="35" t="s">
         <v>56</v>
       </c>
       <c r="J15" s="3" t="s">
@@ -1826,29 +1846,29 @@
       <c r="L15" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="M15" s="26" t="s">
+      <c r="M15" s="25" t="s">
         <v>17</v>
       </c>
       <c r="N15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="O15" s="37" t="s">
+      <c r="O15" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="P15" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="P15" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q15" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="R15" s="12"/>
+      <c r="Q15" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="R15" s="11"/>
       <c r="S15" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:23">
-      <c r="A16" s="31" t="s">
-        <v>71</v>
+      <c r="A16" s="30" t="s">
+        <v>70</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>27</v>
@@ -1865,13 +1885,13 @@
       <c r="F16" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G16" s="33" t="s">
+      <c r="G16" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="H16" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="I16" s="36" t="s">
+      <c r="H16" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="35" t="s">
         <v>56</v>
       </c>
       <c r="J16" s="3" t="s">
@@ -1883,29 +1903,29 @@
       <c r="L16" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="M16" s="26" t="s">
+      <c r="M16" s="25" t="s">
         <v>17</v>
       </c>
       <c r="N16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="O16" s="37" t="s">
+      <c r="O16" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="P16" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="P16" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q16" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="R16" s="12"/>
+      <c r="Q16" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="R16" s="11"/>
       <c r="S16" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:20">
-      <c r="A17" s="37" t="s">
-        <v>72</v>
+      <c r="A17" s="36" t="s">
+        <v>71</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>26</v>
@@ -1922,13 +1942,13 @@
       <c r="F17" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G17" s="33" t="s">
+      <c r="G17" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="H17" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="I17" s="36" t="s">
+      <c r="H17" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="35" t="s">
         <v>56</v>
       </c>
       <c r="J17" s="3" t="s">
@@ -1940,29 +1960,29 @@
       <c r="L17" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="M17" s="26" t="s">
+      <c r="M17" s="25" t="s">
         <v>17</v>
       </c>
       <c r="N17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="O17" s="37" t="s">
+      <c r="O17" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="P17" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="P17" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q17" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="R17" s="12"/>
+      <c r="Q17" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="R17" s="11"/>
       <c r="S17" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:20">
-      <c r="A18" s="31" t="s">
-        <v>73</v>
+      <c r="A18" s="30" t="s">
+        <v>72</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>28</v>
@@ -1979,13 +1999,13 @@
       <c r="F18" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G18" s="33" t="s">
+      <c r="G18" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="H18" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="I18" s="36" t="s">
+      <c r="H18" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="35" t="s">
         <v>56</v>
       </c>
       <c r="J18" s="3" t="s">
@@ -1997,29 +2017,29 @@
       <c r="L18" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="M18" s="26" t="s">
+      <c r="M18" s="25" t="s">
         <v>17</v>
       </c>
       <c r="N18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="O18" s="37" t="s">
+      <c r="O18" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="P18" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="P18" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q18" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="R18" s="12"/>
+      <c r="Q18" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="R18" s="11"/>
       <c r="S18" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:20">
-      <c r="A19" s="37" t="s">
-        <v>74</v>
+      <c r="A19" s="36" t="s">
+        <v>73</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>23</v>
@@ -2036,13 +2056,13 @@
       <c r="F19" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G19" s="33" t="s">
+      <c r="G19" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="H19" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="I19" s="36" t="s">
+      <c r="H19" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" s="35" t="s">
         <v>56</v>
       </c>
       <c r="J19" s="3" t="s">
@@ -2054,449 +2074,449 @@
       <c r="L19" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="M19" s="26" t="s">
+      <c r="M19" s="25" t="s">
         <v>17</v>
       </c>
       <c r="N19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="O19" s="37" t="s">
+      <c r="O19" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="P19" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="P19" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q19" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="R19" s="12"/>
+      <c r="Q19" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="R19" s="11"/>
       <c r="S19" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:20">
-      <c r="A20" s="22"/>
+      <c r="A20" s="21"/>
       <c r="B20" s="4"/>
-      <c r="C20" s="25"/>
+      <c r="C20" s="24"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="15"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="14"/>
       <c r="H20" s="3"/>
-      <c r="I20" s="16"/>
+      <c r="I20" s="15"/>
       <c r="J20" s="3"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="17"/>
-      <c r="M20" s="21"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="20"/>
       <c r="N20" s="3"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="8"/>
-      <c r="Q20" s="11"/>
-      <c r="R20" s="22"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="21"/>
       <c r="S20" s="1"/>
     </row>
     <row r="21" spans="1:20">
-      <c r="A21" s="22"/>
+      <c r="A21" s="21"/>
       <c r="B21" s="4"/>
-      <c r="C21" s="25"/>
+      <c r="C21" s="24"/>
       <c r="D21" s="3"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="15"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="14"/>
       <c r="H21" s="3"/>
-      <c r="I21" s="16"/>
+      <c r="I21" s="15"/>
       <c r="J21" s="3"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="21"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="20"/>
       <c r="N21" s="3"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="8"/>
-      <c r="Q21" s="11"/>
-      <c r="R21" s="22"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="21"/>
       <c r="S21" s="1"/>
     </row>
     <row r="22" spans="1:20">
-      <c r="A22" s="22"/>
+      <c r="A22" s="21"/>
       <c r="B22" s="4"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="15"/>
       <c r="J22" s="3"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="22"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="21"/>
       <c r="N22" s="3"/>
-      <c r="O22" s="22"/>
-      <c r="P22" s="23"/>
-      <c r="Q22" s="24"/>
-      <c r="R22" s="22"/>
+      <c r="O22" s="21"/>
+      <c r="P22" s="22"/>
+      <c r="Q22" s="23"/>
+      <c r="R22" s="21"/>
       <c r="S22" s="1"/>
     </row>
     <row r="23" spans="1:20">
-      <c r="A23" s="22"/>
+      <c r="A23" s="21"/>
       <c r="B23" s="4"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="15"/>
       <c r="J23" s="3"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="22"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="21"/>
       <c r="N23" s="3"/>
-      <c r="O23" s="22"/>
-      <c r="P23" s="23"/>
-      <c r="Q23" s="24"/>
-      <c r="R23" s="22"/>
+      <c r="O23" s="21"/>
+      <c r="P23" s="22"/>
+      <c r="Q23" s="23"/>
+      <c r="R23" s="21"/>
       <c r="S23" s="1"/>
     </row>
     <row r="24" spans="1:20">
-      <c r="A24" s="22"/>
+      <c r="A24" s="21"/>
       <c r="B24" s="4"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="15"/>
       <c r="J24" s="3"/>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17"/>
-      <c r="M24" s="22"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="21"/>
       <c r="N24" s="3"/>
-      <c r="O24" s="22"/>
-      <c r="P24" s="23"/>
-      <c r="Q24" s="24"/>
-      <c r="R24" s="22"/>
+      <c r="O24" s="21"/>
+      <c r="P24" s="22"/>
+      <c r="Q24" s="23"/>
+      <c r="R24" s="21"/>
       <c r="S24" s="1"/>
     </row>
     <row r="25" spans="1:20">
-      <c r="A25" s="22"/>
+      <c r="A25" s="21"/>
       <c r="B25" s="4"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="15"/>
       <c r="J25" s="3"/>
-      <c r="K25" s="17"/>
-      <c r="L25" s="17"/>
-      <c r="M25" s="22"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="21"/>
       <c r="N25" s="3"/>
-      <c r="O25" s="22"/>
-      <c r="P25" s="23"/>
-      <c r="Q25" s="24"/>
-      <c r="R25" s="22"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="22"/>
+      <c r="Q25" s="23"/>
+      <c r="R25" s="21"/>
       <c r="S25" s="1"/>
     </row>
     <row r="26" spans="1:20">
-      <c r="A26" s="22"/>
+      <c r="A26" s="21"/>
       <c r="B26" s="4"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="15"/>
       <c r="J26" s="3"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="17"/>
-      <c r="M26" s="22"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="21"/>
       <c r="N26" s="3"/>
-      <c r="O26" s="22"/>
-      <c r="P26" s="23"/>
-      <c r="Q26" s="24"/>
-      <c r="R26" s="22"/>
+      <c r="O26" s="21"/>
+      <c r="P26" s="22"/>
+      <c r="Q26" s="23"/>
+      <c r="R26" s="21"/>
       <c r="S26" s="1"/>
     </row>
     <row r="27" spans="1:20">
-      <c r="A27" s="22"/>
+      <c r="A27" s="21"/>
       <c r="B27" s="4"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="15"/>
       <c r="J27" s="3"/>
-      <c r="K27" s="17"/>
-      <c r="L27" s="17"/>
-      <c r="M27" s="22"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="21"/>
       <c r="N27" s="3"/>
-      <c r="O27" s="22"/>
-      <c r="P27" s="23"/>
-      <c r="Q27" s="24"/>
-      <c r="R27" s="22"/>
+      <c r="O27" s="21"/>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="23"/>
+      <c r="R27" s="21"/>
       <c r="S27" s="1"/>
     </row>
     <row r="28" spans="1:20">
-      <c r="A28" s="22"/>
+      <c r="A28" s="21"/>
       <c r="B28" s="4"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="15"/>
       <c r="J28" s="3"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="22"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="21"/>
       <c r="N28" s="3"/>
-      <c r="O28" s="22"/>
-      <c r="P28" s="23"/>
-      <c r="Q28" s="24"/>
-      <c r="R28" s="22"/>
+      <c r="O28" s="21"/>
+      <c r="P28" s="22"/>
+      <c r="Q28" s="23"/>
+      <c r="R28" s="21"/>
       <c r="S28" s="1"/>
     </row>
     <row r="29" spans="1:20">
-      <c r="A29" s="22"/>
+      <c r="A29" s="21"/>
       <c r="B29" s="4"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="15"/>
       <c r="J29" s="3"/>
-      <c r="K29" s="17"/>
-      <c r="L29" s="17"/>
-      <c r="M29" s="22"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
+      <c r="M29" s="21"/>
       <c r="N29" s="3"/>
-      <c r="O29" s="22"/>
-      <c r="P29" s="23"/>
-      <c r="Q29" s="24"/>
-      <c r="R29" s="22"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="22"/>
+      <c r="Q29" s="23"/>
+      <c r="R29" s="21"/>
       <c r="S29" s="1"/>
     </row>
     <row r="30" spans="1:20">
-      <c r="A30" s="22"/>
+      <c r="A30" s="21"/>
       <c r="B30" s="4"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="15"/>
       <c r="J30" s="3"/>
-      <c r="K30" s="17"/>
-      <c r="L30" s="17"/>
-      <c r="M30" s="22"/>
+      <c r="K30" s="16"/>
+      <c r="L30" s="16"/>
+      <c r="M30" s="21"/>
       <c r="N30" s="3"/>
-      <c r="O30" s="22"/>
-      <c r="P30" s="23"/>
-      <c r="Q30" s="24"/>
-      <c r="R30" s="22"/>
+      <c r="O30" s="21"/>
+      <c r="P30" s="22"/>
+      <c r="Q30" s="23"/>
+      <c r="R30" s="21"/>
       <c r="S30" s="1"/>
     </row>
     <row r="31" spans="1:20">
-      <c r="A31" s="22"/>
+      <c r="A31" s="21"/>
       <c r="B31" s="4"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="15"/>
       <c r="J31" s="3"/>
-      <c r="K31" s="17"/>
-      <c r="L31" s="17"/>
-      <c r="M31" s="22"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="16"/>
+      <c r="M31" s="21"/>
       <c r="N31" s="3"/>
-      <c r="O31" s="22"/>
-      <c r="P31" s="23"/>
-      <c r="Q31" s="24"/>
-      <c r="R31" s="22"/>
+      <c r="O31" s="21"/>
+      <c r="P31" s="22"/>
+      <c r="Q31" s="23"/>
+      <c r="R31" s="21"/>
       <c r="S31" s="1"/>
     </row>
     <row r="32" spans="1:20">
-      <c r="A32" s="22"/>
+      <c r="A32" s="21"/>
       <c r="B32" s="4"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="15"/>
       <c r="J32" s="3"/>
-      <c r="K32" s="17"/>
-      <c r="L32" s="17"/>
-      <c r="M32" s="22"/>
+      <c r="K32" s="16"/>
+      <c r="L32" s="16"/>
+      <c r="M32" s="21"/>
       <c r="N32" s="3"/>
-      <c r="O32" s="22"/>
-      <c r="P32" s="23"/>
-      <c r="Q32" s="24"/>
-      <c r="R32" s="22"/>
+      <c r="O32" s="21"/>
+      <c r="P32" s="22"/>
+      <c r="Q32" s="23"/>
+      <c r="R32" s="21"/>
       <c r="S32" s="1"/>
-      <c r="T32" s="13"/>
+      <c r="T32" s="12"/>
     </row>
     <row r="33" spans="1:19">
-      <c r="A33" s="22"/>
+      <c r="A33" s="21"/>
       <c r="B33" s="4"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="22"/>
-      <c r="I33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="15"/>
       <c r="J33" s="3"/>
-      <c r="K33" s="17"/>
-      <c r="L33" s="17"/>
-      <c r="M33" s="22"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="21"/>
       <c r="N33" s="3"/>
-      <c r="O33" s="22"/>
-      <c r="P33" s="23"/>
-      <c r="Q33" s="24"/>
-      <c r="R33" s="22"/>
+      <c r="O33" s="21"/>
+      <c r="P33" s="22"/>
+      <c r="Q33" s="23"/>
+      <c r="R33" s="21"/>
       <c r="S33" s="1"/>
     </row>
     <row r="34" spans="1:19">
-      <c r="A34" s="19"/>
+      <c r="A34" s="18"/>
       <c r="B34" s="4"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="18"/>
-      <c r="I34" s="16"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="15"/>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
-      <c r="L34" s="17"/>
-      <c r="M34" s="15"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="14"/>
       <c r="N34" s="3"/>
-      <c r="O34" s="7"/>
-      <c r="P34" s="8"/>
-      <c r="Q34" s="11"/>
-      <c r="R34" s="12"/>
+      <c r="O34" s="6"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="10"/>
+      <c r="R34" s="11"/>
       <c r="S34" s="1"/>
     </row>
     <row r="35" spans="1:19">
-      <c r="A35" s="19"/>
+      <c r="A35" s="18"/>
       <c r="B35" s="4"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="18"/>
-      <c r="I35" s="16"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="15"/>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
-      <c r="L35" s="17"/>
-      <c r="M35" s="15"/>
+      <c r="L35" s="16"/>
+      <c r="M35" s="14"/>
       <c r="N35" s="3"/>
-      <c r="O35" s="7"/>
-      <c r="P35" s="8"/>
-      <c r="Q35" s="11"/>
-      <c r="R35" s="12"/>
+      <c r="O35" s="6"/>
+      <c r="P35" s="7"/>
+      <c r="Q35" s="10"/>
+      <c r="R35" s="11"/>
       <c r="S35" s="1"/>
     </row>
     <row r="36" spans="1:19">
-      <c r="A36" s="19"/>
+      <c r="A36" s="18"/>
       <c r="B36" s="4"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="18"/>
-      <c r="I36" s="16"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="15"/>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
-      <c r="L36" s="17"/>
-      <c r="M36" s="15"/>
+      <c r="L36" s="16"/>
+      <c r="M36" s="14"/>
       <c r="N36" s="3"/>
-      <c r="O36" s="7"/>
-      <c r="P36" s="8"/>
-      <c r="Q36" s="11"/>
-      <c r="R36" s="12"/>
+      <c r="O36" s="6"/>
+      <c r="P36" s="7"/>
+      <c r="Q36" s="10"/>
+      <c r="R36" s="11"/>
       <c r="S36" s="1"/>
     </row>
     <row r="37" spans="1:19">
-      <c r="A37" s="19"/>
+      <c r="A37" s="18"/>
       <c r="B37" s="4"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="18"/>
-      <c r="I37" s="16"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="15"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
-      <c r="L37" s="17"/>
-      <c r="M37" s="15"/>
+      <c r="L37" s="16"/>
+      <c r="M37" s="14"/>
       <c r="N37" s="3"/>
-      <c r="O37" s="7"/>
-      <c r="P37" s="8"/>
-      <c r="Q37" s="11"/>
-      <c r="R37" s="12"/>
+      <c r="O37" s="6"/>
+      <c r="P37" s="7"/>
+      <c r="Q37" s="10"/>
+      <c r="R37" s="11"/>
       <c r="S37" s="1"/>
     </row>
     <row r="38" spans="1:19">
-      <c r="A38" s="19"/>
+      <c r="A38" s="18"/>
       <c r="B38" s="4"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="16"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="15"/>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
-      <c r="L38" s="17"/>
-      <c r="M38" s="15"/>
+      <c r="L38" s="16"/>
+      <c r="M38" s="14"/>
       <c r="N38" s="3"/>
-      <c r="O38" s="7"/>
-      <c r="P38" s="8"/>
-      <c r="Q38" s="11"/>
-      <c r="R38" s="12"/>
+      <c r="O38" s="6"/>
+      <c r="P38" s="7"/>
+      <c r="Q38" s="10"/>
+      <c r="R38" s="11"/>
       <c r="S38" s="1"/>
     </row>
     <row r="39" spans="1:19">
-      <c r="A39" s="19"/>
+      <c r="A39" s="18"/>
       <c r="B39" s="4"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="16"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="15"/>
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
-      <c r="L39" s="17"/>
-      <c r="M39" s="15"/>
+      <c r="L39" s="16"/>
+      <c r="M39" s="14"/>
       <c r="N39" s="3"/>
-      <c r="O39" s="7"/>
-      <c r="P39" s="8"/>
-      <c r="Q39" s="11"/>
-      <c r="R39" s="12"/>
+      <c r="O39" s="6"/>
+      <c r="P39" s="7"/>
+      <c r="Q39" s="10"/>
+      <c r="R39" s="11"/>
       <c r="S39" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="29" type="noConversion"/>
+  <phoneticPr fontId="31" type="noConversion"/>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S39" xr:uid="{53648117-6315-BD4B-95C3-AF9A5887C458}">
       <formula1>"Y,N"</formula1>
@@ -2547,34 +2567,34 @@
       <c r="C3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="24" t="s">
         <v>35</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="I3" s="26" t="s">
+      <c r="I3" s="25" t="s">
         <v>17</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="26" t="s">
+      <c r="K3" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="L3" s="27" t="s">
+      <c r="L3" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="M3" s="28" t="s">
+      <c r="M3" s="27" t="s">
         <v>39</v>
       </c>
       <c r="N3" t="s">

</xml_diff>